<commit_message>
renamed samples to match expression matrix
</commit_message>
<xml_diff>
--- a/input_files/metadata_forcorrWGCNA.xlsx
+++ b/input_files/metadata_forcorrWGCNA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allysondemerlis/Documents/GitHub/woundhealingPdam/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9B7EDB-94ED-5549-9C23-C2F855238DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707FA324-6568-B345-899A-9FF3C19399CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13480" yWindow="500" windowWidth="13100" windowHeight="16180" xr2:uid="{C5B48F37-C1BD-E04E-8808-D7BD29D83388}"/>
+    <workbookView xWindow="15420" yWindow="500" windowWidth="13100" windowHeight="16140" xr2:uid="{C5B48F37-C1BD-E04E-8808-D7BD29D83388}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,78 +41,6 @@
     <t>sample</t>
   </si>
   <si>
-    <t>h0_C1</t>
-  </si>
-  <si>
-    <t>h0_C2</t>
-  </si>
-  <si>
-    <t>h0_C3</t>
-  </si>
-  <si>
-    <t>h0_X</t>
-  </si>
-  <si>
-    <t>h0_Y</t>
-  </si>
-  <si>
-    <t>h0_Z</t>
-  </si>
-  <si>
-    <t>h1_C1</t>
-  </si>
-  <si>
-    <t>h2_C2</t>
-  </si>
-  <si>
-    <t>h1_C2</t>
-  </si>
-  <si>
-    <t>h1_C3</t>
-  </si>
-  <si>
-    <t>h1_X</t>
-  </si>
-  <si>
-    <t>h1_Y</t>
-  </si>
-  <si>
-    <t>h1_Z</t>
-  </si>
-  <si>
-    <t>h2_C1</t>
-  </si>
-  <si>
-    <t>h2_C3</t>
-  </si>
-  <si>
-    <t>h2_X</t>
-  </si>
-  <si>
-    <t>h2_Y</t>
-  </si>
-  <si>
-    <t>h2_Z</t>
-  </si>
-  <si>
-    <t>h4_C1</t>
-  </si>
-  <si>
-    <t>h4_C2</t>
-  </si>
-  <si>
-    <t>h4_C3</t>
-  </si>
-  <si>
-    <t>h4_X</t>
-  </si>
-  <si>
-    <t>h4_Y</t>
-  </si>
-  <si>
-    <t>h4_Z</t>
-  </si>
-  <si>
     <t>hour0_control</t>
   </si>
   <si>
@@ -135,6 +63,78 @@
   </si>
   <si>
     <t>hour4_wounded</t>
+  </si>
+  <si>
+    <t>0301C1</t>
+  </si>
+  <si>
+    <t>0302C2</t>
+  </si>
+  <si>
+    <t>0303C3</t>
+  </si>
+  <si>
+    <t>0304X</t>
+  </si>
+  <si>
+    <t>0305Y</t>
+  </si>
+  <si>
+    <t>0306Z</t>
+  </si>
+  <si>
+    <t>1307C1</t>
+  </si>
+  <si>
+    <t>1308C2</t>
+  </si>
+  <si>
+    <t>1309C3</t>
+  </si>
+  <si>
+    <t>1310X</t>
+  </si>
+  <si>
+    <t>1311Y</t>
+  </si>
+  <si>
+    <t>1312Z</t>
+  </si>
+  <si>
+    <t>2313C1</t>
+  </si>
+  <si>
+    <t>2314C2</t>
+  </si>
+  <si>
+    <t>2315C3</t>
+  </si>
+  <si>
+    <t>2316X</t>
+  </si>
+  <si>
+    <t>2317Y</t>
+  </si>
+  <si>
+    <t>2318Z</t>
+  </si>
+  <si>
+    <t>4325C1</t>
+  </si>
+  <si>
+    <t>4326C2</t>
+  </si>
+  <si>
+    <t>4327C3</t>
+  </si>
+  <si>
+    <t>4328X</t>
+  </si>
+  <si>
+    <t>4329Y</t>
+  </si>
+  <si>
+    <t>4330Z</t>
   </si>
 </sst>
 </file>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327455C2-0BF0-0D4F-B007-1B4441BCAAFF}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,33 +513,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -568,7 +568,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -597,7 +597,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -626,7 +626,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -713,7 +713,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -742,7 +742,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -771,7 +771,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -800,7 +800,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -829,7 +829,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -858,7 +858,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -916,7 +916,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -945,7 +945,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -1090,7 +1090,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -1148,7 +1148,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>

</xml_diff>